<commit_message>
Update code & add data 300, 301, 303, 305
</commit_message>
<xml_diff>
--- a/Nisa/output/data_300.xlsx
+++ b/Nisa/output/data_300.xlsx
@@ -446,87 +446,87 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2015_Maret</t>
+          <t>kalori_2015_Maret</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2015_September</t>
+          <t>kalori_2015_September</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2016_Maret</t>
+          <t>kalori_2016_Maret</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2016_September</t>
+          <t>kalori_2016_September</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2017_Maret</t>
+          <t>kalori_2017_Maret</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2017_September</t>
+          <t>kalori_2017_September</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2018_Maret</t>
+          <t>kalori_2018_Maret</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2018_September</t>
+          <t>kalori_2018_September</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2019_Maret</t>
+          <t>kalori_2019_Maret</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2019_September</t>
+          <t>kalori_2019_September</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2020_Maret</t>
+          <t>kalori_2020_Maret</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2021_Maret</t>
+          <t>kalori_2021_Maret</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2021_September</t>
+          <t>kalori_2021_September</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2022_Maret</t>
+          <t>kalori_2022_Maret</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2022_September</t>
+          <t>kalori_2022_September</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2023_Maret</t>
+          <t>kalori_2023_Maret</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>konsumsi_2024_Maret</t>
+          <t>kalori_2024_Maret</t>
         </is>
       </c>
     </row>

</xml_diff>